<commit_message>
Tests almost finished, only "Taekwondo position" left. After finishing all the tests, I have to copy the table into the documentation.
TODO:
 - write a resume in English and Bulgarian
 - organize and write the CDs for the conf.
</commit_message>
<xml_diff>
--- a/docs/Documentation/Ver 2/Algorithms tests comparison table.xlsx
+++ b/docs/Documentation/Ver 2/Algorithms tests comparison table.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Squat</t>
   </si>
@@ -33,34 +33,34 @@
     <t>Waving with right hand</t>
   </si>
   <si>
-    <t>Right hand punch</t>
-  </si>
-  <si>
-    <t>Left hand punch</t>
-  </si>
-  <si>
-    <t>Jump</t>
-  </si>
-  <si>
     <t>Dynamic time warping</t>
   </si>
   <si>
-    <t>Minimal-Variance matching</t>
-  </si>
-  <si>
     <t>Elastic action comparison with freedom degree</t>
+  </si>
+  <si>
+    <t>Taekwondo position</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -84,7 +84,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -94,6 +94,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,14 +411,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
@@ -414,44 +431,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="G1" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
+      <c r="A2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.91659999999999997</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.71430000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.75570000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>